<commit_message>
spero di non star pushando il mio venv
</commit_message>
<xml_diff>
--- a/ranking_parameters.xlsx
+++ b/ranking_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad28c4a52f214314/Desktop/tic_tac_toe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="8_{0C342675-382D-453B-9EFE-B12C290C7B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E582A86D-49F8-43D1-8B73-C3459EE6B35C}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="8_{0C342675-382D-453B-9EFE-B12C290C7B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B825DFB-027B-4DAA-9A18-5EB045864BB0}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="2244" windowWidth="15744" windowHeight="9708" xr2:uid="{41553A18-C4D9-44C0-BB0D-1AD163D8E2DA}"/>
+    <workbookView minimized="1" xWindow="348" yWindow="2244" windowWidth="15744" windowHeight="9708" xr2:uid="{41553A18-C4D9-44C0-BB0D-1AD163D8E2DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>N_star</t>
   </si>
@@ -56,6 +56,21 @@
   </si>
   <si>
     <t>mean_train_reward</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Q3 - CHOICE OF N_star</t>
+  </si>
+  <si>
+    <t>Q1 - CHOICE OF epsilon</t>
+  </si>
+  <si>
+    <t>Q5 - CHOICE OF eps_opt</t>
+  </si>
+  <si>
+    <t>Q13 - CHOICE OF N_star</t>
   </si>
 </sst>
 </file>
@@ -79,7 +94,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,19 +103,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -120,11 +129,11 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -439,327 +448,409 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24510EAB-5C70-4309-9DBB-A0AAEC3D485A}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="J2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="L2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>0.82399999999999995</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
         <v>0.1</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F3" s="3">
         <v>0.2331</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.88339999999999996</v>
+      </c>
+      <c r="L3">
+        <v>-4.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>0.81699999999999995</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="E3">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>0.2</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>0.1216</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="J4">
+        <v>1000</v>
+      </c>
+      <c r="K4">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="L4">
+        <v>-1.67E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>100</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="4">
         <v>0.90900000000000003</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>0.3</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>2.6100000000000002E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="J5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0.94320000000000004</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>1000</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>0.84299999999999997</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>0.4</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>-9.5399999999999999E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="J6">
+        <v>20000</v>
+      </c>
+      <c r="K6">
+        <v>0.93579999999999997</v>
+      </c>
+      <c r="L6">
+        <v>-0.104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>10000</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>0.84099999999999997</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>0.5</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <v>-0.1603</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="J7">
+        <v>30000</v>
+      </c>
+      <c r="K7">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="L7">
+        <v>-8.9099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>15000</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>0.79600000000000004</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>40000</v>
+      </c>
+      <c r="K8">
+        <v>0.92049999999999998</v>
+      </c>
+      <c r="L8">
+        <v>-0.112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>20000</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>0.76900000000000002</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>30000</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>0.81399999999999995</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>40000</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>0.77100000000000002</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F13" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>-2E-3</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>0.156</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>1</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>0.32700000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>0.2</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>0.54100000000000004</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
         <v>0.61399999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
         <v>0.4</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B17" s="2">
         <v>0.72199999999999998</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
         <v>0.78600000000000003</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F17" s="2">
         <v>100</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>0.372</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
         <v>0.6</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B18" s="6">
         <v>0.85599999999999998</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>-3.0000000000000001E-3</v>
       </c>
-      <c r="D17">
+      <c r="D18">
         <v>0.9</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>1000</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>0.375</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>0.8</v>
-      </c>
-      <c r="B18">
-        <v>0.84899999999999998</v>
-      </c>
-      <c r="C18">
-        <v>-5.0000000000000001E-3</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="F18" s="6">
-        <v>10000</v>
-      </c>
-      <c r="G18" s="6">
-        <v>0.38800000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>1</v>
       </c>
       <c r="B19">
         <v>0.84899999999999998</v>
       </c>
       <c r="C19">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="F19" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.38800000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="C20">
         <v>-0.16700000000000001</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <v>0.88200000000000001</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>15000</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <v>0.36199999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F20">
-        <v>20000</v>
-      </c>
-      <c r="G20">
-        <v>0.252</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F21">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="G21">
-        <v>2.3E-2</v>
+        <v>0.252</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F22">
+        <v>30000</v>
+      </c>
+      <c r="G22">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F23">
         <v>40000</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>-5.7000000000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G23" s="1"/>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>